<commit_message>
won history sars memory level 15~18
</commit_message>
<xml_diff>
--- a/oneshot_from1to14.xlsx
+++ b/oneshot_from1to14.xlsx
@@ -9,15 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27870" windowHeight="9735" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27870" windowHeight="9735" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1 (2)" sheetId="3" r:id="rId2"/>
+    <sheet name="1~14 oneshot" sheetId="1" r:id="rId1"/>
+    <sheet name="1~14 twoshot" sheetId="3" r:id="rId2"/>
+    <sheet name="15~18 oneshot" sheetId="5" r:id="rId3"/>
+    <sheet name="15~18 twoshot" sheetId="4" r:id="rId4"/>
+    <sheet name="15~18 fourshot" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Sheet1 (2)'!$A$1:$E$227</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1~14 oneshot'!$A$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'1~14 twoshot'!$A$1:$E$227</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'15~18 twoshot'!$C$1:$C$29</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="388">
   <si>
     <t>level1</t>
   </si>
@@ -1070,6 +1074,162 @@
   </si>
   <si>
     <t>파란새</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D:\myGit\Angry</t>
+  </si>
+  <si>
+    <t>Birds\kimyibae_AB\python_client\experiences\startAt_20180529_1450_16\level15_shot1_20180529_154140</t>
+  </si>
+  <si>
+    <t>level15</t>
+  </si>
+  <si>
+    <t>angle</t>
+  </si>
+  <si>
+    <t>tap</t>
+  </si>
+  <si>
+    <t>reward</t>
+  </si>
+  <si>
+    <t>Birds\kimyibae_AB\python_client\experiences\startAt_20180529_1450_16\level15_shot0_20180529_154059</t>
+  </si>
+  <si>
+    <t>Birds\kimyibae_AB\python_client\experiences\startAt_20180529_1450_175\level17_shot1_20180529_223521</t>
+  </si>
+  <si>
+    <t>level17</t>
+  </si>
+  <si>
+    <t>Birds\kimyibae_AB\python_client\experiences\startAt_20180529_1450_175\level17_shot0_20180529_223441</t>
+  </si>
+  <si>
+    <t>Birds\kimyibae_AB\python_client\experiences\startAt_20180529_1450_177\level17_shot1_20180529_223830</t>
+  </si>
+  <si>
+    <t>Birds\kimyibae_AB\python_client\experiences\startAt_20180529_1450_177\level17_shot0_20180529_223746</t>
+  </si>
+  <si>
+    <t>Birds\kimyibae_AB\python_client\experiences\startAt_20180529_1450_179\level17_shot1_20180529_224138</t>
+  </si>
+  <si>
+    <t>Birds\kimyibae_AB\python_client\experiences\startAt_20180529_1450_179\level17_shot0_20180529_224052</t>
+  </si>
+  <si>
+    <t>Birds\kimyibae_AB\python_client\experiences\startAt_20180529_1450_180\level17_shot1_20180529_224253</t>
+  </si>
+  <si>
+    <t>Birds\kimyibae_AB\python_client\experiences\startAt_20180529_1450_180\level17_shot0_20180529_224208</t>
+  </si>
+  <si>
+    <t>Birds\kimyibae_AB\python_client\experiences\startAt_20180529_1450_181\level17_shot1_20180529_224408</t>
+  </si>
+  <si>
+    <t>Birds\kimyibae_AB\python_client\experiences\startAt_20180529_1450_181\level17_shot0_20180529_224323</t>
+  </si>
+  <si>
+    <t>Birds\kimyibae_AB\python_client\experiences\startAt_20180529_1450_182\level17_shot1_20180529_224530</t>
+  </si>
+  <si>
+    <t>Birds\kimyibae_AB\python_client\experiences\startAt_20180529_1450_182\level17_shot0_20180529_224443</t>
+  </si>
+  <si>
+    <t>Birds\kimyibae_AB\python_client\experiences\startAt_20180529_1450_185\level17_shot1_20180529_225027</t>
+  </si>
+  <si>
+    <t>Birds\kimyibae_AB\python_client\experiences\startAt_20180529_1450_185\level17_shot0_20180529_224940</t>
+  </si>
+  <si>
+    <t>Birds\kimyibae_AB\python_client\experiences\startAt_20180529_1450_189\level17_shot1_20180529_225708</t>
+  </si>
+  <si>
+    <t>Birds\kimyibae_AB\python_client\experiences\startAt_20180529_1450_189\level17_shot0_20180529_225623</t>
+  </si>
+  <si>
+    <t>Birds\kimyibae_AB\python_client\experiences\startAt_20180529_1450_30\level15_shot1_20180529_161445</t>
+  </si>
+  <si>
+    <t>Birds\kimyibae_AB\python_client\experiences\startAt_20180529_1450_30\level15_shot0_20180529_161351</t>
+  </si>
+  <si>
+    <t>Birds\kimyibae_AB\python_client\experiences\startAt_20180529_1450_55\level15_shot1_20180529_171858</t>
+  </si>
+  <si>
+    <t>Birds\kimyibae_AB\python_client\experiences\startAt_20180529_1450_55\level15_shot0_20180529_171814</t>
+  </si>
+  <si>
+    <t>Birds\kimyibae_AB\python_client\experiences\startAt_20180529_1450_57\level15_shot1_20180529_172256</t>
+  </si>
+  <si>
+    <t>Birds\kimyibae_AB\python_client\experiences\startAt_20180529_1450_57\level15_shot0_20180529_172213</t>
+  </si>
+  <si>
+    <t>Birds\kimyibae_AB\python_client\experiences\startAt_20180529_1450_59\level15_shot1_20180529_172655</t>
+  </si>
+  <si>
+    <t>Birds\kimyibae_AB\python_client\experiences\startAt_20180529_1450_59\level15_shot0_20180529_172613</t>
+  </si>
+  <si>
+    <t>Birds\kimyibae_AB\python_client\experiences\startAt_20180529_1450_99\level16_shot1_20180529_191315</t>
+  </si>
+  <si>
+    <t>level16</t>
+  </si>
+  <si>
+    <t>Birds\kimyibae_AB\python_client\experiences\startAt_20180529_1450_99\level16_shot0_20180529_191228</t>
+  </si>
+  <si>
+    <t>level</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>angle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reward</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Birds\kimyibae_AB\python_client\experiences\startAt_20180529_1450_103\level16_shot0_20180529_192253</t>
+  </si>
+  <si>
+    <t>내거에서</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>level15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>level15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shot1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shot0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shot0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shot1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shot2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shot3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3420,8 +3580,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:E227"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B239" sqref="B239"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E221" sqref="E221"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -7303,4 +7463,821 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5"/>
+  <cols>
+    <col min="1" max="1" width="15.375" customWidth="1"/>
+    <col min="2" max="2" width="101" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="1" customFormat="1">
+      <c r="A1" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="E1" s="1">
+        <v>26</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="G1" s="1">
+        <v>1800</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="I1" s="1">
+        <v>67720</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:G33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5"/>
+  <cols>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="101.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="B1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C1" t="s">
+        <v>375</v>
+      </c>
+      <c r="D1" t="s">
+        <v>376</v>
+      </c>
+      <c r="E1" t="s">
+        <v>331</v>
+      </c>
+      <c r="F1" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="D2" s="2">
+        <v>25</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1700</v>
+      </c>
+      <c r="F2" s="2">
+        <v>41480</v>
+      </c>
+      <c r="G2">
+        <f>SUM(F2:F3)</f>
+        <v>44430</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="D3" s="2">
+        <v>20</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1800</v>
+      </c>
+      <c r="F3" s="2">
+        <v>2950</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="D4" s="1">
+        <v>36</v>
+      </c>
+      <c r="E4" s="1">
+        <v>2000</v>
+      </c>
+      <c r="F4" s="1">
+        <v>34730</v>
+      </c>
+      <c r="G4" s="1">
+        <f>SUM(F4:F5)</f>
+        <v>51280</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="D5" s="1">
+        <v>34</v>
+      </c>
+      <c r="E5" s="1">
+        <v>600</v>
+      </c>
+      <c r="F5" s="1">
+        <v>16550</v>
+      </c>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>340</v>
+      </c>
+      <c r="B6" t="s">
+        <v>366</v>
+      </c>
+      <c r="C6" t="s">
+        <v>342</v>
+      </c>
+      <c r="D6">
+        <v>67</v>
+      </c>
+      <c r="E6">
+        <v>800</v>
+      </c>
+      <c r="F6">
+        <v>28390</v>
+      </c>
+      <c r="G6">
+        <f>SUM(F6:F7)</f>
+        <v>47390</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>340</v>
+      </c>
+      <c r="B7" t="s">
+        <v>367</v>
+      </c>
+      <c r="C7" t="s">
+        <v>342</v>
+      </c>
+      <c r="D7">
+        <v>59</v>
+      </c>
+      <c r="E7">
+        <v>500</v>
+      </c>
+      <c r="F7">
+        <v>19000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>340</v>
+      </c>
+      <c r="B8" t="s">
+        <v>368</v>
+      </c>
+      <c r="C8" t="s">
+        <v>342</v>
+      </c>
+      <c r="D8">
+        <v>67</v>
+      </c>
+      <c r="E8">
+        <v>1700</v>
+      </c>
+      <c r="F8">
+        <v>28200</v>
+      </c>
+      <c r="G8">
+        <f>SUM(F8:F9)</f>
+        <v>46060</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>340</v>
+      </c>
+      <c r="B9" t="s">
+        <v>369</v>
+      </c>
+      <c r="C9" t="s">
+        <v>342</v>
+      </c>
+      <c r="D9">
+        <v>61</v>
+      </c>
+      <c r="E9">
+        <v>1800</v>
+      </c>
+      <c r="F9">
+        <v>17860</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>340</v>
+      </c>
+      <c r="B10" t="s">
+        <v>370</v>
+      </c>
+      <c r="C10" t="s">
+        <v>342</v>
+      </c>
+      <c r="D10">
+        <v>72</v>
+      </c>
+      <c r="E10">
+        <v>800</v>
+      </c>
+      <c r="F10">
+        <v>26240</v>
+      </c>
+      <c r="G10">
+        <f>SUM(F10:F11)</f>
+        <v>44400</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>340</v>
+      </c>
+      <c r="B11" t="s">
+        <v>371</v>
+      </c>
+      <c r="C11" t="s">
+        <v>342</v>
+      </c>
+      <c r="D11">
+        <v>63</v>
+      </c>
+      <c r="E11">
+        <v>1100</v>
+      </c>
+      <c r="F11">
+        <v>18160</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" hidden="1">
+      <c r="A12" t="s">
+        <v>340</v>
+      </c>
+      <c r="B12" t="s">
+        <v>372</v>
+      </c>
+      <c r="C12" t="s">
+        <v>373</v>
+      </c>
+      <c r="D12">
+        <v>23</v>
+      </c>
+      <c r="E12">
+        <v>1100</v>
+      </c>
+      <c r="F12">
+        <v>51390</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" hidden="1">
+      <c r="A13" t="s">
+        <v>340</v>
+      </c>
+      <c r="B13" t="s">
+        <v>374</v>
+      </c>
+      <c r="C13" t="s">
+        <v>373</v>
+      </c>
+      <c r="D13">
+        <v>22</v>
+      </c>
+      <c r="E13">
+        <v>1200</v>
+      </c>
+      <c r="F13">
+        <v>11470</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="2" customFormat="1">
+      <c r="A14" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D14" s="2">
+        <v>25</v>
+      </c>
+      <c r="E14" s="2">
+        <v>1600</v>
+      </c>
+      <c r="F14" s="2">
+        <v>40090</v>
+      </c>
+      <c r="G14" s="2">
+        <f>SUM(F14:F15)</f>
+        <v>41020</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="2" customFormat="1">
+      <c r="A15" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D15" s="2">
+        <v>17</v>
+      </c>
+      <c r="E15" s="2">
+        <v>900</v>
+      </c>
+      <c r="F15" s="2">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>340</v>
+      </c>
+      <c r="B16" t="s">
+        <v>350</v>
+      </c>
+      <c r="C16" t="s">
+        <v>348</v>
+      </c>
+      <c r="D16">
+        <v>23</v>
+      </c>
+      <c r="E16">
+        <v>1100</v>
+      </c>
+      <c r="F16">
+        <v>24710</v>
+      </c>
+      <c r="G16">
+        <f>SUM(F16:F17)</f>
+        <v>47080</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" t="s">
+        <v>340</v>
+      </c>
+      <c r="B17" t="s">
+        <v>351</v>
+      </c>
+      <c r="C17" t="s">
+        <v>348</v>
+      </c>
+      <c r="D17">
+        <v>19</v>
+      </c>
+      <c r="E17">
+        <v>600</v>
+      </c>
+      <c r="F17">
+        <v>22370</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" t="s">
+        <v>340</v>
+      </c>
+      <c r="B18" t="s">
+        <v>352</v>
+      </c>
+      <c r="C18" t="s">
+        <v>348</v>
+      </c>
+      <c r="D18">
+        <v>23</v>
+      </c>
+      <c r="E18">
+        <v>1000</v>
+      </c>
+      <c r="F18">
+        <v>25020</v>
+      </c>
+      <c r="G18">
+        <f>SUM(F18:F19)</f>
+        <v>49670</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" t="s">
+        <v>340</v>
+      </c>
+      <c r="B19" t="s">
+        <v>353</v>
+      </c>
+      <c r="C19" t="s">
+        <v>348</v>
+      </c>
+      <c r="D19">
+        <v>21</v>
+      </c>
+      <c r="E19">
+        <v>1100</v>
+      </c>
+      <c r="F19">
+        <v>24650</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" t="s">
+        <v>340</v>
+      </c>
+      <c r="B20" t="s">
+        <v>354</v>
+      </c>
+      <c r="C20" t="s">
+        <v>348</v>
+      </c>
+      <c r="D20">
+        <v>29</v>
+      </c>
+      <c r="E20">
+        <v>1800</v>
+      </c>
+      <c r="F20">
+        <v>23950</v>
+      </c>
+      <c r="G20">
+        <f>SUM(F20:F21)</f>
+        <v>45090</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" t="s">
+        <v>340</v>
+      </c>
+      <c r="B21" t="s">
+        <v>355</v>
+      </c>
+      <c r="C21" t="s">
+        <v>348</v>
+      </c>
+      <c r="D21">
+        <v>22</v>
+      </c>
+      <c r="E21">
+        <v>500</v>
+      </c>
+      <c r="F21">
+        <v>21140</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" t="s">
+        <v>340</v>
+      </c>
+      <c r="B22" t="s">
+        <v>356</v>
+      </c>
+      <c r="C22" t="s">
+        <v>348</v>
+      </c>
+      <c r="D22">
+        <v>27</v>
+      </c>
+      <c r="E22">
+        <v>2100</v>
+      </c>
+      <c r="F22">
+        <v>20260</v>
+      </c>
+      <c r="G22">
+        <f>SUM(F22:F23)</f>
+        <v>49640</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" t="s">
+        <v>340</v>
+      </c>
+      <c r="B23" t="s">
+        <v>357</v>
+      </c>
+      <c r="C23" t="s">
+        <v>348</v>
+      </c>
+      <c r="D23">
+        <v>23</v>
+      </c>
+      <c r="E23">
+        <v>1200</v>
+      </c>
+      <c r="F23">
+        <v>29380</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" t="s">
+        <v>340</v>
+      </c>
+      <c r="B24" t="s">
+        <v>358</v>
+      </c>
+      <c r="C24" t="s">
+        <v>348</v>
+      </c>
+      <c r="D24">
+        <v>30</v>
+      </c>
+      <c r="E24">
+        <v>1700</v>
+      </c>
+      <c r="F24">
+        <v>26870</v>
+      </c>
+      <c r="G24">
+        <f>SUM(F24:F25)</f>
+        <v>48980</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" t="s">
+        <v>340</v>
+      </c>
+      <c r="B25" t="s">
+        <v>359</v>
+      </c>
+      <c r="C25" t="s">
+        <v>348</v>
+      </c>
+      <c r="D25">
+        <v>24</v>
+      </c>
+      <c r="E25">
+        <v>1800</v>
+      </c>
+      <c r="F25">
+        <v>22110</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" t="s">
+        <v>340</v>
+      </c>
+      <c r="B26" t="s">
+        <v>360</v>
+      </c>
+      <c r="C26" t="s">
+        <v>348</v>
+      </c>
+      <c r="D26">
+        <v>30</v>
+      </c>
+      <c r="E26">
+        <v>1800</v>
+      </c>
+      <c r="F26">
+        <v>19470</v>
+      </c>
+      <c r="G26">
+        <f>SUM(F26:F27)</f>
+        <v>49790</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" t="s">
+        <v>340</v>
+      </c>
+      <c r="B27" t="s">
+        <v>361</v>
+      </c>
+      <c r="C27" t="s">
+        <v>348</v>
+      </c>
+      <c r="D27">
+        <v>27</v>
+      </c>
+      <c r="E27">
+        <v>1500</v>
+      </c>
+      <c r="F27">
+        <v>30320</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="D28" s="1">
+        <v>30</v>
+      </c>
+      <c r="E28" s="1">
+        <v>1600</v>
+      </c>
+      <c r="F28" s="1">
+        <v>29760</v>
+      </c>
+      <c r="G28" s="1">
+        <f>SUM(F28:F29)</f>
+        <v>50490</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="D29" s="1">
+        <v>31</v>
+      </c>
+      <c r="E29" s="1">
+        <v>1900</v>
+      </c>
+      <c r="F29" s="1">
+        <v>20730</v>
+      </c>
+      <c r="G29" s="1"/>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="B32" t="s">
+        <v>382</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="D32" s="1">
+        <v>52</v>
+      </c>
+      <c r="E32" s="1">
+        <v>1700</v>
+      </c>
+      <c r="F32" s="1">
+        <f>48310-F33</f>
+        <v>33320</v>
+      </c>
+      <c r="G32">
+        <f>SUM(F32:F33)</f>
+        <v>48310</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6">
+      <c r="B33" t="s">
+        <v>383</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="D33" s="1">
+        <v>52</v>
+      </c>
+      <c r="E33" s="1">
+        <v>2400</v>
+      </c>
+      <c r="F33" s="1">
+        <v>14990</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="C1:C29">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="level15"/>
+        <filter val="level17"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <sortState ref="A2:F57">
+    <sortCondition ref="C2"/>
+  </sortState>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="H1:J4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetData>
+    <row r="1" spans="8:10">
+      <c r="H1" t="s">
+        <v>384</v>
+      </c>
+      <c r="I1">
+        <v>16</v>
+      </c>
+      <c r="J1">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="2" spans="8:10">
+      <c r="H2" t="s">
+        <v>385</v>
+      </c>
+      <c r="I2">
+        <v>27</v>
+      </c>
+      <c r="J2">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="3" spans="8:10">
+      <c r="H3" t="s">
+        <v>386</v>
+      </c>
+      <c r="I3">
+        <v>27</v>
+      </c>
+      <c r="J3">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="4" spans="8:10">
+      <c r="H4" t="s">
+        <v>387</v>
+      </c>
+      <c r="I4">
+        <v>25</v>
+      </c>
+      <c r="J4">
+        <v>500</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>